<commit_message>
fixed bug on data summary report
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Acinetobacter species" sheetId="1" r:id="rId1"/>
-    <sheet name="Pseudomonas aeruginosa" sheetId="11" r:id="rId2"/>
+    <sheet name="Acinetobacter_species" sheetId="1" r:id="rId1"/>
+    <sheet name="Pseudomonas_aeruginosa" sheetId="11" r:id="rId2"/>
     <sheet name="Beta-Hemolytic Streptococci" sheetId="2" r:id="rId3"/>
     <sheet name="Burkholderia cepacia" sheetId="3" r:id="rId4"/>
     <sheet name="ENTEROBACTERIACEAE_X_SAL_SHI" sheetId="4" r:id="rId5"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="A2:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4779,11 +4779,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -5684,10 +5687,13 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S579" sqref="S579"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
new patch for the report
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Acinetobacter_species_v2" sheetId="20" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="178">
   <si>
     <t>Acinetobacter species</t>
   </si>
@@ -563,6 +563,15 @@
   </si>
   <si>
     <t>Doripenem</t>
+  </si>
+  <si>
+    <t>PEN_ND10</t>
+  </si>
+  <si>
+    <t>PEN_NM</t>
+  </si>
+  <si>
+    <t>LVX_NM</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1251,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,18 +1583,26 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -1613,8 +1630,17 @@
       <c r="I1" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1642,8 +1668,17 @@
       <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="12">
+        <v>8</v>
+      </c>
+      <c r="L2" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1669,8 +1704,14 @@
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1696,8 +1737,14 @@
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1714,17 +1761,21 @@
         <v>5</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="2">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L5" s="12">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1752,8 +1803,17 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J6" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1781,8 +1841,17 @@
       <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J7" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K7" s="12">
+        <v>16</v>
+      </c>
+      <c r="L7" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1810,8 +1879,17 @@
       <c r="I8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J8" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -1837,8 +1915,14 @@
       <c r="I9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J9" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1864,8 +1948,14 @@
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J10" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1891,8 +1981,14 @@
       <c r="I11" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J11" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1917,6 +2013,29 @@
       </c>
       <c r="I12" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="L12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="17">
+        <v>24</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new fix for data summary report
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Acinetobacter_species_v2" sheetId="20" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Vibrio cholerae" sheetId="17" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ENTEROBACTERIACEAE_X_SAL_SHI!$J$1:$J$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ENTEROBACTERIACEAE_X_SAL_SHI!$A$1:$L$23</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -1585,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -8253,12 +8253,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="12"/>
@@ -8307,22 +8308,22 @@
         <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
@@ -8331,13 +8332,13 @@
         <v>5</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="K2" s="12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L2" s="12">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8345,10 +8346,10 @@
         <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -8357,10 +8358,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="2">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
@@ -8369,13 +8370,13 @@
         <v>5</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="K3" s="12">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="L3" s="12">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8383,23 +8384,23 @@
         <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>17</v>
       </c>
-      <c r="G4" s="2">
-        <v>21</v>
-      </c>
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
@@ -8407,13 +8408,13 @@
         <v>5</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="K4" s="12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L4" s="12">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8421,22 +8422,22 @@
         <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="2">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>5</v>
@@ -8445,13 +8446,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="K5" s="12">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L5" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8459,31 +8460,27 @@
         <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2">
-        <v>19</v>
-      </c>
-      <c r="G6" s="2">
-        <v>23</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K6" s="12">
         <v>8</v>
@@ -8497,22 +8494,22 @@
         <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>5</v>
@@ -8521,13 +8518,13 @@
         <v>5</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K7" s="12">
         <v>16</v>
       </c>
       <c r="L7" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8535,19 +8532,19 @@
         <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2">
         <v>18</v>
@@ -8559,7 +8556,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="K8" s="12">
         <v>32</v>
@@ -8573,22 +8570,22 @@
         <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2">
-        <v>19</v>
-      </c>
       <c r="G9" s="2">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>5</v>
@@ -8597,13 +8594,13 @@
         <v>5</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K9" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L9" s="12">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8611,37 +8608,31 @@
         <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2">
-        <v>17</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="K10" s="12">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L10" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8649,22 +8640,22 @@
         <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>5</v>
@@ -8673,13 +8664,13 @@
         <v>5</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="K11" s="12">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L11" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8687,22 +8678,22 @@
         <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>5</v>
@@ -8711,13 +8702,13 @@
         <v>5</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K12" s="12">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L12" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8725,22 +8716,22 @@
         <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="2">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>5</v>
@@ -8749,13 +8740,13 @@
         <v>5</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="K13" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L13" s="12">
-        <v>0.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8763,22 +8754,22 @@
         <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G14" s="2">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>5</v>
@@ -8787,13 +8778,13 @@
         <v>5</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="K14" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L14" s="12">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8801,22 +8792,22 @@
         <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="F15" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>5</v>
@@ -8825,13 +8816,13 @@
         <v>5</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="K15" s="12">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="L15" s="12">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8839,22 +8830,22 @@
         <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="F16" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G16" s="2">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>5</v>
@@ -8863,13 +8854,7 @@
         <v>5</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="K16" s="12">
-        <v>2</v>
-      </c>
-      <c r="L16" s="12">
-        <v>0.5</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8877,33 +8862,37 @@
         <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="F17" s="2">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2">
+        <v>18</v>
+      </c>
       <c r="H17" s="2" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K17" s="12">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L17" s="12">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -8949,13 +8938,13 @@
         <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
@@ -8973,7 +8962,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K19" s="12">
         <v>4</v>
@@ -8987,22 +8976,22 @@
         <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>5</v>
@@ -9011,13 +9000,13 @@
         <v>5</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K20" s="12">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="L20" s="12">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -9025,22 +9014,22 @@
         <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F21" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G21" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>5</v>
@@ -9049,7 +9038,13 @@
         <v>5</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="K21" s="12">
+        <v>128</v>
+      </c>
+      <c r="L21" s="12">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -9057,37 +9052,37 @@
         <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" s="12">
+        <v>4</v>
+      </c>
+      <c r="L22" s="12">
         <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2">
-        <v>14</v>
-      </c>
-      <c r="G22" s="2">
-        <v>17</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" s="12">
-        <v>64</v>
-      </c>
-      <c r="L22" s="12">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -9095,31 +9090,37 @@
         <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="2">
         <v>17</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="2"/>
+      <c r="G23" s="2">
+        <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="I23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="K23" s="12">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="L23" s="12">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -9134,6 +9135,11 @@
       <c r="I24" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L23">
+    <sortState ref="A2:L23">
+      <sortCondition ref="C1:C23"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>